<commit_message>
Ressources design + Avancée design + Modif SQL Structure
</commit_message>
<xml_diff>
--- a/.my_folder/DataBase_Structure_CV.xlsx
+++ b/.my_folder/DataBase_Structure_CV.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Thomas_Dev\WorldGT\01_cv_classic_php\ZZZ_my_folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev_Projets\WorldGT\01_cv_classic_php\.my_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6184BE0C-DF47-448C-A147-6209C82D76E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1795C6F-6CE5-4CAC-9BAA-2E7180E9E53B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="203">
   <si>
     <t>languages</t>
   </si>
@@ -54,9 +54,6 @@
     <t>id_contact</t>
   </si>
   <si>
-    <t>Level</t>
-  </si>
-  <si>
     <t>Details</t>
   </si>
   <si>
@@ -435,9 +432,6 @@
     <t>Quelles Technologies utilisées dans l'expérience</t>
   </si>
   <si>
-    <t xml:space="preserve">cv_name </t>
-  </si>
-  <si>
     <t xml:space="preserve">cv_title </t>
   </si>
   <si>
@@ -628,6 +622,18 @@
   </si>
   <si>
     <t>id_exp_pro_skill</t>
+  </si>
+  <si>
+    <t>is_current_job</t>
+  </si>
+  <si>
+    <t>cecrl_level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cv_abrv </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cv_category </t>
   </si>
 </sst>
 </file>
@@ -862,7 +868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1028,9 +1034,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1334,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH50"/>
+  <dimension ref="A1:AH51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G1048576"/>
+      <selection activeCell="B16" sqref="B16:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1389,7 +1392,7 @@
       <c r="F1" s="33"/>
       <c r="G1" s="11"/>
       <c r="H1" s="27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I1" s="34"/>
       <c r="J1" s="10"/>
@@ -1398,14 +1401,14 @@
       </c>
       <c r="L1" s="32"/>
       <c r="N1" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P1" s="10"/>
       <c r="Q1" s="27" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="R1" s="34"/>
       <c r="T1" s="25" t="s">
@@ -1413,7 +1416,7 @@
       </c>
       <c r="U1" s="26"/>
       <c r="W1" s="41" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="X1" s="48"/>
       <c r="Y1" s="10"/>
@@ -1421,7 +1424,7 @@
         <v>1</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.35">
@@ -1429,241 +1432,241 @@
         <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="X2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Z2" s="10">
         <v>2</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Z3" s="10">
         <v>3</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J4" s="10">
         <v>1</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="O4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="O4" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="Q4" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V4" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="W4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X4" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Z4" s="10">
         <v>4</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" s="10">
         <v>2</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S5" s="10"/>
       <c r="T5" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="U5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V5" s="10"/>
       <c r="W5" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="X5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z5" s="10">
         <v>5</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1671,328 +1674,328 @@
         <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" s="10">
         <v>3</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S6" s="10"/>
       <c r="T6" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V6" s="10"/>
       <c r="W6" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z6" s="10">
         <v>6</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S7" s="10"/>
       <c r="T7" s="6" t="s">
-        <v>48</v>
+        <v>199</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="V7" s="10"/>
       <c r="W7" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Z7" s="10">
         <v>7</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="11"/>
       <c r="K8" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L8" s="29" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S8" s="10"/>
-      <c r="T8" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="U8" s="8" t="s">
-        <v>13</v>
+      <c r="T8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="V8" s="10"/>
       <c r="W8" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="X8" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Z8" s="10">
         <v>8</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E9" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="27" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I9" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="K9" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="K9" s="12" t="s">
-        <v>170</v>
-      </c>
       <c r="L9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S9" s="10"/>
-      <c r="T9" s="14" t="s">
-        <v>92</v>
+      <c r="T9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="U9" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="V9" s="10"/>
       <c r="W9" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Z9" s="10">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>9</v>
+        <v>200</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S10" s="10"/>
-      <c r="T10" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="U10" s="35" t="s">
-        <v>167</v>
+      <c r="T10" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="V10" s="10"/>
       <c r="W10" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="X10" s="42" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Z10" s="10">
         <v>10</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:34" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="10"/>
       <c r="B11" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S11" s="10"/>
-      <c r="T11" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="U11" s="5" t="s">
-        <v>16</v>
+      <c r="T11" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="U11" s="35" t="s">
+        <v>165</v>
       </c>
       <c r="V11" s="10"/>
       <c r="W11" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="X11" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Y11" s="10"/>
       <c r="Z11" s="10">
         <v>11</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
@@ -2004,542 +2007,537 @@
     </row>
     <row r="12" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="H12" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="T12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="T12" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="V12" s="10"/>
+      <c r="W12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="X12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z12" s="10">
+        <v>12</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="L13" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="N13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="U12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="W12" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="X12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z12" s="10">
-        <v>12</v>
-      </c>
-      <c r="AA12" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="16" t="s">
+      <c r="O13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="R13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="T13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="U13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="W13" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="X13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z13" s="10"/>
+    </row>
+    <row r="14" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="F13" s="30" t="s">
-        <v>168</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="L13" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="R13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="T13" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="U13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="W13" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="X13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z13" s="10"/>
-    </row>
-    <row r="14" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E14" s="17" t="s">
-        <v>111</v>
-      </c>
       <c r="F14" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q14" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="R14" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S14" s="11">
         <v>6</v>
       </c>
-      <c r="V14" s="11">
-        <v>6</v>
+      <c r="T14" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="U14" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="45"/>
       <c r="E15" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H15" s="53" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I15" s="54"/>
       <c r="J15" s="10">
         <v>9</v>
       </c>
       <c r="K15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="V15" s="11">
+        <v>6</v>
+      </c>
+      <c r="W15" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="X15" s="49" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E16" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="L15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="O15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="T15" s="25" t="s">
+      <c r="F16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q16" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="R16" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="T16" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="U16" s="36" t="s">
+        <v>165</v>
+      </c>
+      <c r="W16" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="U15" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="W15" s="41" t="s">
+      <c r="X16" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="45"/>
+      <c r="E17" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q17" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="T17" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="X15" s="49" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="4" t="s">
+      <c r="U17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="W17" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="X17" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K16" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="N16" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="O16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q16" s="27" t="s">
-        <v>154</v>
-      </c>
-      <c r="R16" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="T16" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="U16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="W16" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="X16" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q17" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="R17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="T17" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="U17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="W17" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="X17" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="56" t="s">
-        <v>186</v>
-      </c>
       <c r="I18" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K18" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L18" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="N18" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O18" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="R18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="T18" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="U18" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="T18" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="U18" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="W18" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="X18" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="E19" s="38" t="s">
         <v>6</v>
       </c>
       <c r="F19" s="39"/>
-      <c r="H19" s="56" t="s">
-        <v>193</v>
+      <c r="H19" s="6" t="s">
+        <v>191</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N19" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q19" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="R19" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="T19" s="14" t="s">
-        <v>148</v>
+        <v>15</v>
+      </c>
+      <c r="T19" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="U19" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="W19" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="31" t="s">
-        <v>168</v>
+      <c r="B20" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="T20" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="T20" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="W20" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="X20" s="49" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N21" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q21" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="R21" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="T21" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="U21" s="36" t="s">
+        <v>165</v>
+      </c>
+      <c r="W21" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="U20" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="W20" s="41" t="s">
+      <c r="X21" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="53" t="s">
+        <v>185</v>
+      </c>
+      <c r="I22" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="K22" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N22" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="O22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q22" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="R22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="T22" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="X20" s="49" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="21" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K21" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N21" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="O21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q21" s="27" t="s">
-        <v>155</v>
-      </c>
-      <c r="R21" s="28" t="s">
-        <v>166</v>
-      </c>
-      <c r="T21" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="U21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="W21" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="X21" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" s="53" t="s">
-        <v>187</v>
-      </c>
-      <c r="I22" s="55" t="s">
-        <v>168</v>
-      </c>
-      <c r="K22" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="N22" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="O22" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q22" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="R22" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="T22" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="U22" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="W22" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="X22" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="9" t="s">
-        <v>90</v>
+      <c r="B23" s="17" t="s">
+        <v>102</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G23" s="10">
         <v>4</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="R23" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="T23" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="U23" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="T23" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="U23" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="W23" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X23" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>16</v>
+      <c r="B24" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K24" s="19" t="s">
         <v>5</v>
@@ -2549,519 +2547,533 @@
         <v>7</v>
       </c>
       <c r="Q24" s="13" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="R24" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="T24" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="U24" s="15"/>
+        <v>15</v>
+      </c>
+      <c r="T24" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="U24" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="W24" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X24" s="15"/>
     </row>
     <row r="25" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E25" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M25" s="10"/>
-      <c r="T25" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="U25" s="35" t="s">
-        <v>166</v>
-      </c>
+      <c r="T25" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="U25" s="15"/>
       <c r="W25" s="41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="X25" s="42" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="Y25" s="10">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="50" t="s">
-        <v>122</v>
-      </c>
-      <c r="C26" s="51" t="s">
-        <v>146</v>
-      </c>
-      <c r="D26" s="10">
-        <v>12</v>
+      <c r="B26" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M26" s="10"/>
       <c r="Q26" s="27" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="R26" s="28" t="s">
-        <v>168</v>
-      </c>
-      <c r="T26" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="U26" s="5" t="s">
-        <v>16</v>
+        <v>166</v>
+      </c>
+      <c r="T26" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="U26" s="35" t="s">
+        <v>164</v>
       </c>
       <c r="W26" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="X26" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="E27" s="38" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F27" s="40" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M27" s="10"/>
       <c r="Q27" s="17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="R27" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S27" s="10"/>
-      <c r="T27" s="9" t="s">
-        <v>35</v>
+      <c r="T27" s="12" t="s">
+        <v>195</v>
       </c>
       <c r="U27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="V27" s="10"/>
+        <v>15</v>
+      </c>
       <c r="W27" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="X27" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>15</v>
+      <c r="B28" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" s="51" t="s">
+        <v>144</v>
+      </c>
+      <c r="D28" s="10">
+        <v>12</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="I28" s="58"/>
+        <v>15</v>
+      </c>
+      <c r="H28" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="I28" s="57"/>
       <c r="K28" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M28" s="10"/>
       <c r="Q28" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R28" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S28" s="10"/>
-      <c r="T28" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="U28" s="8" t="s">
-        <v>16</v>
+      <c r="T28" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="U28" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="V28" s="10"/>
       <c r="W28" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="X28" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="46" t="s">
-        <v>127</v>
-      </c>
-      <c r="C29" s="47" t="s">
+      <c r="B29" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M29" s="10"/>
       <c r="Q29" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="R29" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="T29" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="U29" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="V29" s="10"/>
     </row>
     <row r="30" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="E30" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M30" s="10"/>
       <c r="Q30" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="R30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="T30" s="25" t="s">
-        <v>199</v>
-      </c>
-      <c r="U30" s="35" t="s">
-        <v>166</v>
+        <v>15</v>
       </c>
       <c r="W30" s="41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="X30" s="42" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="Y30" s="10">
         <v>11</v>
       </c>
     </row>
     <row r="31" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M31" s="10"/>
+      <c r="T31" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="U31" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="W31" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="X31" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H32" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K32" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="L32" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="M32" s="10"/>
+      <c r="T32" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="U32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="W32" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="X32" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="50" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="K33" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M33" s="10"/>
+      <c r="T33" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="U33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="W33" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="X33" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B34" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="C31" s="52" t="s">
-        <v>168</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M31" s="10"/>
-      <c r="T31" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="U31" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="W31" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="X31" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K32" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="L32" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="M32" s="10"/>
-      <c r="T32" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="U32" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="W32" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="X32" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K33" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="L33" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M33" s="10"/>
-      <c r="T33" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="U33" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="W33" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="X33" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="9" t="s">
-        <v>130</v>
-      </c>
       <c r="C34" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H34" s="57" t="s">
-        <v>93</v>
-      </c>
-      <c r="I34" s="59" t="s">
-        <v>168</v>
+        <v>15</v>
+      </c>
+      <c r="H34" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="I34" s="58" t="s">
+        <v>166</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M34" s="10"/>
       <c r="Q34" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="T34" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="U34" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>16</v>
+      <c r="B35" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K35" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M35" s="10"/>
       <c r="Q35" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="R35" s="35" t="s">
-        <v>147</v>
-      </c>
-      <c r="T35" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="U35" s="35" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="W35" s="41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="X35" s="42" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B36" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="H36" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K36" s="18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M36" s="10"/>
       <c r="Q36" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R36" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S36" s="10"/>
-      <c r="T36" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="U36" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="V36" s="10"/>
+      <c r="T36" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="U36" s="35" t="s">
+        <v>164</v>
+      </c>
       <c r="W36" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="X36" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="2:31" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B37" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="H37" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q37" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R37" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="T37" s="9" t="s">
-        <v>35</v>
+        <v>15</v>
+      </c>
+      <c r="T37" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="U37" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="V37" s="10"/>
       <c r="W37" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="X37" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H38" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q38" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R38" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="T38" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="U38" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="T38" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="U38" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="W38" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X38" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I39" s="1"/>
       <c r="Q39" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R39" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="T39" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="U39" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="2:31" x14ac:dyDescent="0.35">
       <c r="I40" s="1"/>
     </row>
-    <row r="47" spans="2:31" x14ac:dyDescent="0.35">
-      <c r="C47" s="1"/>
-    </row>
     <row r="48" spans="2:31" x14ac:dyDescent="0.35">
-      <c r="C48" s="1"/>
       <c r="AC48" s="11"/>
       <c r="AE48" s="1"/>
     </row>
@@ -3071,8 +3083,12 @@
       <c r="AE49" s="1"/>
     </row>
     <row r="50" spans="3:31" x14ac:dyDescent="0.35">
+      <c r="C50" s="1"/>
       <c r="AC50" s="11"/>
       <c r="AE50" s="1"/>
+    </row>
+    <row r="51" spans="3:31" x14ac:dyDescent="0.35">
+      <c r="C51" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>